<commit_message>
Fix dashboard to exclude auto-closed breaks from statistics
- Exclude breaks with 'Auto-closed', 'force-closed', 'System' in reason
- Cap break duration at 120 minutes (anything over is likely an error)
- Applied to: get_realtime_metrics, get_break_distribution_today, get_agent_performance_today

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/database/2026-01/break_logs_2026-01-27.xlsx
+++ b/database/2026-01/break_logs_2026-01-27.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H140"/>
+  <dimension ref="A1:H154"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5063,6 +5063,466 @@
       </c>
       <c r="H140" t="inlineStr"/>
     </row>
+    <row r="141">
+      <c r="A141" t="n">
+        <v>7025939006</v>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>Booster_lav</t>
+        </is>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>🎀 𝒽𝒾_𝓁𝒶𝒶𝓋 🎀</t>
+        </is>
+      </c>
+      <c r="D141" t="inlineStr">
+        <is>
+          <t>🚻 Comfort Room</t>
+        </is>
+      </c>
+      <c r="E141" t="inlineStr">
+        <is>
+          <t>OUT</t>
+        </is>
+      </c>
+      <c r="F141" t="inlineStr">
+        <is>
+          <t>2026-01-27 10:27:29</t>
+        </is>
+      </c>
+      <c r="G141" t="inlineStr"/>
+      <c r="H141" t="inlineStr"/>
+    </row>
+    <row r="142">
+      <c r="A142" t="n">
+        <v>7025939006</v>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>Booster_lav</t>
+        </is>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>🎀 𝒽𝒾_𝓁𝒶𝒶𝓋 🎀</t>
+        </is>
+      </c>
+      <c r="D142" t="inlineStr">
+        <is>
+          <t>🚻 Comfort Room</t>
+        </is>
+      </c>
+      <c r="E142" t="inlineStr">
+        <is>
+          <t>BACK</t>
+        </is>
+      </c>
+      <c r="F142" t="inlineStr">
+        <is>
+          <t>2026-01-27 10:31:11</t>
+        </is>
+      </c>
+      <c r="G142" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="H142" t="inlineStr"/>
+    </row>
+    <row r="143">
+      <c r="A143" t="n">
+        <v>8313813326</v>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>booster_roxan</t>
+        </is>
+      </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>roxy</t>
+        </is>
+      </c>
+      <c r="D143" t="inlineStr">
+        <is>
+          <t>🚻 Comfort Room</t>
+        </is>
+      </c>
+      <c r="E143" t="inlineStr">
+        <is>
+          <t>BACK</t>
+        </is>
+      </c>
+      <c r="F143" t="inlineStr">
+        <is>
+          <t>2026-01-27 10:33:02</t>
+        </is>
+      </c>
+      <c r="G143" t="n">
+        <v>185.5</v>
+      </c>
+      <c r="H143" t="inlineStr"/>
+    </row>
+    <row r="144">
+      <c r="A144" t="n">
+        <v>8397936341</v>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>Booster_Moja</t>
+        </is>
+      </c>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t>ʍօʝǟ🔫🔥</t>
+        </is>
+      </c>
+      <c r="D144" t="inlineStr">
+        <is>
+          <t>🚬 Smoke Break</t>
+        </is>
+      </c>
+      <c r="E144" t="inlineStr">
+        <is>
+          <t>OUT</t>
+        </is>
+      </c>
+      <c r="F144" t="inlineStr">
+        <is>
+          <t>2026-01-27 11:00:02</t>
+        </is>
+      </c>
+      <c r="G144" t="inlineStr"/>
+      <c r="H144" t="inlineStr"/>
+    </row>
+    <row r="145">
+      <c r="A145" t="n">
+        <v>8203583816</v>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>Cyrus0228</t>
+        </is>
+      </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>Cyrus Rufo</t>
+        </is>
+      </c>
+      <c r="D145" t="inlineStr">
+        <is>
+          <t>🚬 Smoke Break</t>
+        </is>
+      </c>
+      <c r="E145" t="inlineStr">
+        <is>
+          <t>OUT</t>
+        </is>
+      </c>
+      <c r="F145" t="inlineStr">
+        <is>
+          <t>2026-01-27 11:02:44</t>
+        </is>
+      </c>
+      <c r="G145" t="inlineStr"/>
+      <c r="H145" t="inlineStr"/>
+    </row>
+    <row r="146">
+      <c r="A146" t="n">
+        <v>8224136102</v>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>Matiluk</t>
+        </is>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>Boost-Lo</t>
+        </is>
+      </c>
+      <c r="D146" t="inlineStr">
+        <is>
+          <t>🚬 Smoke Break</t>
+        </is>
+      </c>
+      <c r="E146" t="inlineStr">
+        <is>
+          <t>OUT</t>
+        </is>
+      </c>
+      <c r="F146" t="inlineStr">
+        <is>
+          <t>2026-01-27 14:31:20</t>
+        </is>
+      </c>
+      <c r="G146" t="inlineStr"/>
+      <c r="H146" t="inlineStr"/>
+    </row>
+    <row r="147">
+      <c r="A147" t="n">
+        <v>8224136102</v>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>Matiluk</t>
+        </is>
+      </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>Boost-Lo</t>
+        </is>
+      </c>
+      <c r="D147" t="inlineStr">
+        <is>
+          <t>🚬 Smoke Break</t>
+        </is>
+      </c>
+      <c r="E147" t="inlineStr">
+        <is>
+          <t>BACK</t>
+        </is>
+      </c>
+      <c r="F147" t="inlineStr">
+        <is>
+          <t>2026-01-27 14:31:24</t>
+        </is>
+      </c>
+      <c r="G147" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H147" t="inlineStr"/>
+    </row>
+    <row r="148">
+      <c r="A148" t="n">
+        <v>8224136102</v>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>Matiluk</t>
+        </is>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>Boost-Lo</t>
+        </is>
+      </c>
+      <c r="D148" t="inlineStr">
+        <is>
+          <t>🚻 Comfort Room</t>
+        </is>
+      </c>
+      <c r="E148" t="inlineStr">
+        <is>
+          <t>OUT</t>
+        </is>
+      </c>
+      <c r="F148" t="inlineStr">
+        <is>
+          <t>2026-01-27 15:36:06</t>
+        </is>
+      </c>
+      <c r="G148" t="inlineStr"/>
+      <c r="H148" t="inlineStr"/>
+    </row>
+    <row r="149">
+      <c r="A149" t="n">
+        <v>8224136102</v>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>Matiluk</t>
+        </is>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>Boost-Lo</t>
+        </is>
+      </c>
+      <c r="D149" t="inlineStr">
+        <is>
+          <t>🚻 Comfort Room</t>
+        </is>
+      </c>
+      <c r="E149" t="inlineStr">
+        <is>
+          <t>BACK</t>
+        </is>
+      </c>
+      <c r="F149" t="inlineStr">
+        <is>
+          <t>2026-01-27 16:41:26</t>
+        </is>
+      </c>
+      <c r="G149" t="n">
+        <v>65.3</v>
+      </c>
+      <c r="H149" t="inlineStr"/>
+    </row>
+    <row r="150">
+      <c r="A150" t="n">
+        <v>8013843575</v>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>Booster_yham</t>
+        </is>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>yham</t>
+        </is>
+      </c>
+      <c r="D150" t="inlineStr">
+        <is>
+          <t>🚬 Smoke Break</t>
+        </is>
+      </c>
+      <c r="E150" t="inlineStr">
+        <is>
+          <t>OUT</t>
+        </is>
+      </c>
+      <c r="F150" t="inlineStr">
+        <is>
+          <t>2026-01-27 18:37:50</t>
+        </is>
+      </c>
+      <c r="G150" t="inlineStr"/>
+      <c r="H150" t="inlineStr"/>
+    </row>
+    <row r="151">
+      <c r="A151" t="n">
+        <v>8013843575</v>
+      </c>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t>Booster_yham</t>
+        </is>
+      </c>
+      <c r="C151" t="inlineStr">
+        <is>
+          <t>yham</t>
+        </is>
+      </c>
+      <c r="D151" t="inlineStr">
+        <is>
+          <t>🚬 Smoke Break</t>
+        </is>
+      </c>
+      <c r="E151" t="inlineStr">
+        <is>
+          <t>BACK</t>
+        </is>
+      </c>
+      <c r="F151" t="inlineStr">
+        <is>
+          <t>2026-01-27 18:55:54</t>
+        </is>
+      </c>
+      <c r="G151" t="n">
+        <v>18.1</v>
+      </c>
+      <c r="H151" t="inlineStr"/>
+    </row>
+    <row r="152">
+      <c r="A152" t="n">
+        <v>8011222190</v>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>syintel</t>
+        </is>
+      </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>Sheena</t>
+        </is>
+      </c>
+      <c r="D152" t="inlineStr">
+        <is>
+          <t>🚻 Comfort Room</t>
+        </is>
+      </c>
+      <c r="E152" t="inlineStr">
+        <is>
+          <t>OUT</t>
+        </is>
+      </c>
+      <c r="F152" t="inlineStr">
+        <is>
+          <t>2026-01-27 20:39:06</t>
+        </is>
+      </c>
+      <c r="G152" t="inlineStr"/>
+      <c r="H152" t="inlineStr"/>
+    </row>
+    <row r="153">
+      <c r="A153" t="n">
+        <v>8011222190</v>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>syintel</t>
+        </is>
+      </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>Sheena</t>
+        </is>
+      </c>
+      <c r="D153" t="inlineStr">
+        <is>
+          <t>🚻 Comfort Room</t>
+        </is>
+      </c>
+      <c r="E153" t="inlineStr">
+        <is>
+          <t>BACK</t>
+        </is>
+      </c>
+      <c r="F153" t="inlineStr">
+        <is>
+          <t>2026-01-27 20:42:17</t>
+        </is>
+      </c>
+      <c r="G153" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="H153" t="inlineStr"/>
+    </row>
+    <row r="154">
+      <c r="A154" t="n">
+        <v>8011222190</v>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>syintel</t>
+        </is>
+      </c>
+      <c r="C154" t="inlineStr">
+        <is>
+          <t>Sheena</t>
+        </is>
+      </c>
+      <c r="D154" t="inlineStr">
+        <is>
+          <t>🚻 Comfort Room</t>
+        </is>
+      </c>
+      <c r="E154" t="inlineStr">
+        <is>
+          <t>OUT</t>
+        </is>
+      </c>
+      <c r="F154" t="inlineStr">
+        <is>
+          <t>2026-01-27 21:27:40</t>
+        </is>
+      </c>
+      <c r="G154" t="inlineStr"/>
+      <c r="H154" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>